<commit_message>
modified:   Acessos.xlsx 	modified:   __pycache__/saves.cpython-313.pyc 	modified:   __pycache__/utilidades.cpython-313.pyc 	modified:   main.py
</commit_message>
<xml_diff>
--- a/Acessos.xlsx
+++ b/Acessos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,6 +825,66 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MARCOSVIN</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>VINICIUS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>DE JESUS LIMA</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>23</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>RUPILOTT22@</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>farjc97</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>luiz</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>fernando</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>cunha</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>28</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>abcdefg12@</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>